<commit_message>
More LaTeX code in excel files
</commit_message>
<xml_diff>
--- a/data/edu_comp_es.xlsx
+++ b/data/edu_comp_es.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV-main\ESP\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031A2E52-41B0-4EDE-821A-92D08382D8F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AAE75F-4680-4730-8409-0341AC8D49B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2790" yWindow="4365" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>what</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Coursera (MOOC platform)</t>
   </si>
   <si>
-    <t>Promedio: 97/100</t>
-  </si>
-  <si>
     <t>University of Dundee</t>
   </si>
   <si>
@@ -58,7 +55,7 @@
     <t>Practical Machine Learning</t>
   </si>
   <si>
-    <t>Certificado: https://www.coursera.org/account/accomplishments/verify/DC7ULMJ3CZWM</t>
+    <t>Promedio: 97/100 (ver \href{https://www.coursera.org/account/accomplishments/verify/DC7ULMJ3CZWM}{certificado})</t>
   </si>
 </sst>
 </file>
@@ -542,9 +539,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -900,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,7 +930,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>2021</v>
@@ -946,26 +942,21 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
         <v>2012</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>